<commit_message>
Correção de modelo massivo de solicitação de acesso a usuário; Funcionalidade de argumentos para Cardapio;
</commit_message>
<xml_diff>
--- a/wwwroot/files/Modelo_Solicitar_Acesso_Massivo.xlsx
+++ b/wwwroot/files/Modelo_Solicitar_Acesso_Massivo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://telefonicacorp-my.sharepoint.com/personal/jhonny_melo_telefonica_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A0151191\repo\Shared_Razor_Components\wwwroot\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E0100370-08F7-4D16-9381-D6A5CD34C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15375705-94A4-4908-9ADD-B5E87988E0E7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B644D487-A696-4196-B608-E7324D705C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="17430" windowHeight="11385" xr2:uid="{6A4CED72-FD60-4E64-A367-6A5DDD467AB0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6A4CED72-FD60-4E64-A367-6A5DDD467AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Acessos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>EMAIL</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>PE085-21</t>
+  </si>
+  <si>
+    <t>TELEFONE</t>
+  </si>
+  <si>
+    <t>(99) 99999-9999</t>
   </si>
 </sst>
 </file>
@@ -273,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -306,6 +312,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -322,10 +331,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,31 +630,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8122E9F5-B166-4BCB-B0B1-864CCB4D7FF3}">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="7" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="7" customWidth="1"/>
-    <col min="12" max="12" width="29.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" hidden="1"/>
+    <col min="7" max="7" width="30.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.1796875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="7" customWidth="1"/>
+    <col min="13" max="13" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -671,23 +677,26 @@
       <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -710,24 +719,27 @@
       <c r="G2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="3">
-        <f>IF(K2&lt;&gt;"",VLOOKUP(K2,DADOS!$D:$E,2,0),"")</f>
+      <c r="K2" s="3">
+        <f>IF(L2&lt;&gt;"",VLOOKUP(L2,DADOS!$D:$E,2,0),"")</f>
         <v>1</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -750,24 +762,27 @@
       <c r="G3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="3">
-        <f>IF(K3&lt;&gt;"",VLOOKUP(K3,DADOS!$D:$E,2,0),"")</f>
+      <c r="K3" s="3">
+        <f>IF(L3&lt;&gt;"",VLOOKUP(L3,DADOS!$D:$E,2,0),"")</f>
         <v>1</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -790,24 +805,27 @@
       <c r="G4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="3">
-        <f>IF(K4&lt;&gt;"",VLOOKUP(K4,DADOS!$D:$E,2,0),"")</f>
+      <c r="K4" s="3">
+        <f>IF(L4&lt;&gt;"",VLOOKUP(L4,DADOS!$D:$E,2,0),"")</f>
         <v>1</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -830,980 +848,983 @@
       <c r="G5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="3">
-        <f>IF(K5&lt;&gt;"",VLOOKUP(K5,DADOS!$D:$E,2,0),"")</f>
+      <c r="K5" s="3">
+        <f>IF(L5&lt;&gt;"",VLOOKUP(L5,DADOS!$D:$E,2,0),"")</f>
         <v>1</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E6" s="2" t="str">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J6" s="3" t="str">
-        <f>IF(K6&lt;&gt;"",VLOOKUP(K6,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="3" t="str">
+        <f>IF(L6&lt;&gt;"",VLOOKUP(L6,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E7" s="2" t="str">
         <f>IF(F7&lt;&gt;"",VLOOKUP(F7,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J7" s="3" t="str">
-        <f>IF(K7&lt;&gt;"",VLOOKUP(K7,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="3" t="str">
+        <f>IF(L7&lt;&gt;"",VLOOKUP(L7,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E8" s="2" t="str">
         <f>IF(F8&lt;&gt;"",VLOOKUP(F8,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J8" s="3" t="str">
-        <f>IF(K8&lt;&gt;"",VLOOKUP(K8,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="3" t="str">
+        <f>IF(L8&lt;&gt;"",VLOOKUP(L8,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E9" s="2" t="str">
         <f>IF(F9&lt;&gt;"",VLOOKUP(F9,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J9" s="3" t="str">
-        <f>IF(K9&lt;&gt;"",VLOOKUP(K9,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="3" t="str">
+        <f>IF(L9&lt;&gt;"",VLOOKUP(L9,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E10" s="2" t="str">
         <f>IF(F10&lt;&gt;"",VLOOKUP(F10,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J10" s="3" t="str">
-        <f>IF(K10&lt;&gt;"",VLOOKUP(K10,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="3" t="str">
+        <f>IF(L10&lt;&gt;"",VLOOKUP(L10,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E11" s="2" t="str">
         <f>IF(F11&lt;&gt;"",VLOOKUP(F11,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J11" s="3" t="str">
-        <f>IF(K11&lt;&gt;"",VLOOKUP(K11,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="3" t="str">
+        <f>IF(L11&lt;&gt;"",VLOOKUP(L11,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E12" s="2" t="str">
         <f>IF(F12&lt;&gt;"",VLOOKUP(F12,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J12" s="3" t="str">
-        <f>IF(K12&lt;&gt;"",VLOOKUP(K12,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="3" t="str">
+        <f>IF(L12&lt;&gt;"",VLOOKUP(L12,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E13" s="2" t="str">
         <f>IF(F13&lt;&gt;"",VLOOKUP(F13,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J13" s="3" t="str">
-        <f>IF(K13&lt;&gt;"",VLOOKUP(K13,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="3" t="str">
+        <f>IF(L13&lt;&gt;"",VLOOKUP(L13,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E14" s="2" t="str">
         <f>IF(F14&lt;&gt;"",VLOOKUP(F14,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J14" s="3" t="str">
-        <f>IF(K14&lt;&gt;"",VLOOKUP(K14,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="str">
+        <f>IF(L14&lt;&gt;"",VLOOKUP(L14,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E15" s="2" t="str">
         <f>IF(F15&lt;&gt;"",VLOOKUP(F15,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J15" s="3" t="str">
-        <f>IF(K15&lt;&gt;"",VLOOKUP(K15,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="3" t="str">
+        <f>IF(L15&lt;&gt;"",VLOOKUP(L15,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E16" s="2" t="str">
         <f>IF(F16&lt;&gt;"",VLOOKUP(F16,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J16" s="3" t="str">
-        <f>IF(K16&lt;&gt;"",VLOOKUP(K16,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="3" t="str">
+        <f>IF(L16&lt;&gt;"",VLOOKUP(L16,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="2" t="str">
         <f>IF(F17&lt;&gt;"",VLOOKUP(F17,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J17" s="3" t="str">
-        <f>IF(K17&lt;&gt;"",VLOOKUP(K17,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="3" t="str">
+        <f>IF(L17&lt;&gt;"",VLOOKUP(L17,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E18" s="2" t="str">
         <f>IF(F18&lt;&gt;"",VLOOKUP(F18,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J18" s="3" t="str">
-        <f>IF(K18&lt;&gt;"",VLOOKUP(K18,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="3" t="str">
+        <f>IF(L18&lt;&gt;"",VLOOKUP(L18,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E19" s="2" t="str">
         <f>IF(F19&lt;&gt;"",VLOOKUP(F19,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J19" s="3" t="str">
-        <f>IF(K19&lt;&gt;"",VLOOKUP(K19,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="3" t="str">
+        <f>IF(L19&lt;&gt;"",VLOOKUP(L19,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E20" s="2" t="str">
         <f>IF(F20&lt;&gt;"",VLOOKUP(F20,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J20" s="3" t="str">
-        <f>IF(K20&lt;&gt;"",VLOOKUP(K20,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="str">
+        <f>IF(L20&lt;&gt;"",VLOOKUP(L20,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E21" s="2" t="str">
         <f>IF(F21&lt;&gt;"",VLOOKUP(F21,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J21" s="3" t="str">
-        <f>IF(K21&lt;&gt;"",VLOOKUP(K21,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="str">
+        <f>IF(L21&lt;&gt;"",VLOOKUP(L21,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E22" s="2" t="str">
         <f>IF(F22&lt;&gt;"",VLOOKUP(F22,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J22" s="3" t="str">
-        <f>IF(K22&lt;&gt;"",VLOOKUP(K22,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="3" t="str">
+        <f>IF(L22&lt;&gt;"",VLOOKUP(L22,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E23" s="2" t="str">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J23" s="3" t="str">
-        <f>IF(K23&lt;&gt;"",VLOOKUP(K23,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="3" t="str">
+        <f>IF(L23&lt;&gt;"",VLOOKUP(L23,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E24" s="2" t="str">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J24" s="3" t="str">
-        <f>IF(K24&lt;&gt;"",VLOOKUP(K24,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="3" t="str">
+        <f>IF(L24&lt;&gt;"",VLOOKUP(L24,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E25" s="2" t="str">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J25" s="3" t="str">
-        <f>IF(K25&lt;&gt;"",VLOOKUP(K25,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="3" t="str">
+        <f>IF(L25&lt;&gt;"",VLOOKUP(L25,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E26" s="2" t="str">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J26" s="3" t="str">
-        <f>IF(K26&lt;&gt;"",VLOOKUP(K26,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="3" t="str">
+        <f>IF(L26&lt;&gt;"",VLOOKUP(L26,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E27" s="2" t="str">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J27" s="3" t="str">
-        <f>IF(K27&lt;&gt;"",VLOOKUP(K27,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="3" t="str">
+        <f>IF(L27&lt;&gt;"",VLOOKUP(L27,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E28" s="2" t="str">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J28" s="3" t="str">
-        <f>IF(K28&lt;&gt;"",VLOOKUP(K28,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="3" t="str">
+        <f>IF(L28&lt;&gt;"",VLOOKUP(L28,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E29" s="2" t="str">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J29" s="3" t="str">
-        <f>IF(K29&lt;&gt;"",VLOOKUP(K29,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="3" t="str">
+        <f>IF(L29&lt;&gt;"",VLOOKUP(L29,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E30" s="2" t="str">
         <f>IF(F30&lt;&gt;"",VLOOKUP(F30,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J30" s="3" t="str">
-        <f>IF(K30&lt;&gt;"",VLOOKUP(K30,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="3" t="str">
+        <f>IF(L30&lt;&gt;"",VLOOKUP(L30,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E31" s="2" t="str">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J31" s="3" t="str">
-        <f>IF(K31&lt;&gt;"",VLOOKUP(K31,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="3" t="str">
+        <f>IF(L31&lt;&gt;"",VLOOKUP(L31,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E32" s="2" t="str">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J32" s="3" t="str">
-        <f>IF(K32&lt;&gt;"",VLOOKUP(K32,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="3" t="str">
+        <f>IF(L32&lt;&gt;"",VLOOKUP(L32,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33" s="2" t="str">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J33" s="3" t="str">
-        <f>IF(K33&lt;&gt;"",VLOOKUP(K33,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="3" t="str">
+        <f>IF(L33&lt;&gt;"",VLOOKUP(L33,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34" s="2" t="str">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J34" s="3" t="str">
-        <f>IF(K34&lt;&gt;"",VLOOKUP(K34,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="3" t="str">
+        <f>IF(L34&lt;&gt;"",VLOOKUP(L34,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35" s="2" t="str">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J35" s="3" t="str">
-        <f>IF(K35&lt;&gt;"",VLOOKUP(K35,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="3" t="str">
+        <f>IF(L35&lt;&gt;"",VLOOKUP(L35,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36" s="2" t="str">
         <f>IF(F36&lt;&gt;"",VLOOKUP(F36,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J36" s="3" t="str">
-        <f>IF(K36&lt;&gt;"",VLOOKUP(K36,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="3" t="str">
+        <f>IF(L36&lt;&gt;"",VLOOKUP(L36,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37" s="2" t="str">
         <f>IF(F37&lt;&gt;"",VLOOKUP(F37,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J37" s="3" t="str">
-        <f>IF(K37&lt;&gt;"",VLOOKUP(K37,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="3" t="str">
+        <f>IF(L37&lt;&gt;"",VLOOKUP(L37,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38" s="2" t="str">
         <f>IF(F38&lt;&gt;"",VLOOKUP(F38,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J38" s="3" t="str">
-        <f>IF(K38&lt;&gt;"",VLOOKUP(K38,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="3" t="str">
+        <f>IF(L38&lt;&gt;"",VLOOKUP(L38,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39" s="2" t="str">
         <f>IF(F39&lt;&gt;"",VLOOKUP(F39,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J39" s="3" t="str">
-        <f>IF(K39&lt;&gt;"",VLOOKUP(K39,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="3" t="str">
+        <f>IF(L39&lt;&gt;"",VLOOKUP(L39,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40" s="2" t="str">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J40" s="3" t="str">
-        <f>IF(K40&lt;&gt;"",VLOOKUP(K40,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="3" t="str">
+        <f>IF(L40&lt;&gt;"",VLOOKUP(L40,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41" s="2" t="str">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J41" s="3" t="str">
-        <f>IF(K41&lt;&gt;"",VLOOKUP(K41,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="3" t="str">
+        <f>IF(L41&lt;&gt;"",VLOOKUP(L41,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42" s="2" t="str">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J42" s="3" t="str">
-        <f>IF(K42&lt;&gt;"",VLOOKUP(K42,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="3" t="str">
+        <f>IF(L42&lt;&gt;"",VLOOKUP(L42,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43" s="2" t="str">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J43" s="3" t="str">
-        <f>IF(K43&lt;&gt;"",VLOOKUP(K43,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="3" t="str">
+        <f>IF(L43&lt;&gt;"",VLOOKUP(L43,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44" s="2" t="str">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J44" s="3" t="str">
-        <f>IF(K44&lt;&gt;"",VLOOKUP(K44,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="3" t="str">
+        <f>IF(L44&lt;&gt;"",VLOOKUP(L44,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45" s="2" t="str">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J45" s="3" t="str">
-        <f>IF(K45&lt;&gt;"",VLOOKUP(K45,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="3" t="str">
+        <f>IF(L45&lt;&gt;"",VLOOKUP(L45,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46" s="2" t="str">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J46" s="3" t="str">
-        <f>IF(K46&lt;&gt;"",VLOOKUP(K46,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="3" t="str">
+        <f>IF(L46&lt;&gt;"",VLOOKUP(L46,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47" s="2" t="str">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J47" s="3" t="str">
-        <f>IF(K47&lt;&gt;"",VLOOKUP(K47,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="3" t="str">
+        <f>IF(L47&lt;&gt;"",VLOOKUP(L47,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48" s="2" t="str">
         <f>IF(F48&lt;&gt;"",VLOOKUP(F48,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J48" s="3" t="str">
-        <f>IF(K48&lt;&gt;"",VLOOKUP(K48,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="3" t="str">
+        <f>IF(L48&lt;&gt;"",VLOOKUP(L48,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="2" t="str">
         <f>IF(F49&lt;&gt;"",VLOOKUP(F49,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J49" s="3" t="str">
-        <f>IF(K49&lt;&gt;"",VLOOKUP(K49,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="3" t="str">
+        <f>IF(L49&lt;&gt;"",VLOOKUP(L49,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="2" t="str">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J50" s="3" t="str">
-        <f>IF(K50&lt;&gt;"",VLOOKUP(K50,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="3" t="str">
+        <f>IF(L50&lt;&gt;"",VLOOKUP(L50,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E51" s="2" t="str">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J51" s="3" t="str">
-        <f>IF(K51&lt;&gt;"",VLOOKUP(K51,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="3" t="str">
+        <f>IF(L51&lt;&gt;"",VLOOKUP(L51,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E52" s="2" t="str">
         <f>IF(F52&lt;&gt;"",VLOOKUP(F52,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J52" s="3" t="str">
-        <f>IF(K52&lt;&gt;"",VLOOKUP(K52,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="3" t="str">
+        <f>IF(L52&lt;&gt;"",VLOOKUP(L52,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E53" s="2" t="str">
         <f>IF(F53&lt;&gt;"",VLOOKUP(F53,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J53" s="3" t="str">
-        <f>IF(K53&lt;&gt;"",VLOOKUP(K53,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="3" t="str">
+        <f>IF(L53&lt;&gt;"",VLOOKUP(L53,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E54" s="2" t="str">
         <f>IF(F54&lt;&gt;"",VLOOKUP(F54,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J54" s="3" t="str">
-        <f>IF(K54&lt;&gt;"",VLOOKUP(K54,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="3" t="str">
+        <f>IF(L54&lt;&gt;"",VLOOKUP(L54,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E55" s="2" t="str">
         <f>IF(F55&lt;&gt;"",VLOOKUP(F55,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J55" s="3" t="str">
-        <f>IF(K55&lt;&gt;"",VLOOKUP(K55,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="3" t="str">
+        <f>IF(L55&lt;&gt;"",VLOOKUP(L55,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E56" s="2" t="str">
         <f>IF(F56&lt;&gt;"",VLOOKUP(F56,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J56" s="3" t="str">
-        <f>IF(K56&lt;&gt;"",VLOOKUP(K56,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="3" t="str">
+        <f>IF(L56&lt;&gt;"",VLOOKUP(L56,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E57" s="2" t="str">
         <f>IF(F57&lt;&gt;"",VLOOKUP(F57,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J57" s="3" t="str">
-        <f>IF(K57&lt;&gt;"",VLOOKUP(K57,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="3" t="str">
+        <f>IF(L57&lt;&gt;"",VLOOKUP(L57,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E58" s="2" t="str">
         <f>IF(F58&lt;&gt;"",VLOOKUP(F58,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J58" s="3" t="str">
-        <f>IF(K58&lt;&gt;"",VLOOKUP(K58,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="3" t="str">
+        <f>IF(L58&lt;&gt;"",VLOOKUP(L58,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E59" s="2" t="str">
         <f>IF(F59&lt;&gt;"",VLOOKUP(F59,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J59" s="3" t="str">
-        <f>IF(K59&lt;&gt;"",VLOOKUP(K59,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3" t="str">
+        <f>IF(L59&lt;&gt;"",VLOOKUP(L59,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E60" s="2" t="str">
         <f>IF(F60&lt;&gt;"",VLOOKUP(F60,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J60" s="3" t="str">
-        <f>IF(K60&lt;&gt;"",VLOOKUP(K60,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="3" t="str">
+        <f>IF(L60&lt;&gt;"",VLOOKUP(L60,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E61" s="2" t="str">
         <f>IF(F61&lt;&gt;"",VLOOKUP(F61,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J61" s="3" t="str">
-        <f>IF(K61&lt;&gt;"",VLOOKUP(K61,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="3" t="str">
+        <f>IF(L61&lt;&gt;"",VLOOKUP(L61,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E62" s="2" t="str">
         <f>IF(F62&lt;&gt;"",VLOOKUP(F62,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J62" s="3" t="str">
-        <f>IF(K62&lt;&gt;"",VLOOKUP(K62,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="3" t="str">
+        <f>IF(L62&lt;&gt;"",VLOOKUP(L62,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E63" s="2" t="str">
         <f>IF(F63&lt;&gt;"",VLOOKUP(F63,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J63" s="3" t="str">
-        <f>IF(K63&lt;&gt;"",VLOOKUP(K63,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="3" t="str">
+        <f>IF(L63&lt;&gt;"",VLOOKUP(L63,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E64" s="2" t="str">
         <f>IF(F64&lt;&gt;"",VLOOKUP(F64,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J64" s="3" t="str">
-        <f>IF(K64&lt;&gt;"",VLOOKUP(K64,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="3" t="str">
+        <f>IF(L64&lt;&gt;"",VLOOKUP(L64,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E65" s="2" t="str">
         <f>IF(F65&lt;&gt;"",VLOOKUP(F65,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J65" s="3" t="str">
-        <f>IF(K65&lt;&gt;"",VLOOKUP(K65,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="3" t="str">
+        <f>IF(L65&lt;&gt;"",VLOOKUP(L65,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E66" s="2" t="str">
         <f>IF(F66&lt;&gt;"",VLOOKUP(F66,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J66" s="3" t="str">
-        <f>IF(K66&lt;&gt;"",VLOOKUP(K66,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="3" t="str">
+        <f>IF(L66&lt;&gt;"",VLOOKUP(L66,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E67" s="2" t="str">
         <f>IF(F67&lt;&gt;"",VLOOKUP(F67,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J67" s="3" t="str">
-        <f>IF(K67&lt;&gt;"",VLOOKUP(K67,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="3" t="str">
+        <f>IF(L67&lt;&gt;"",VLOOKUP(L67,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E68" s="2" t="str">
         <f>IF(F68&lt;&gt;"",VLOOKUP(F68,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J68" s="3" t="str">
-        <f>IF(K68&lt;&gt;"",VLOOKUP(K68,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="3" t="str">
+        <f>IF(L68&lt;&gt;"",VLOOKUP(L68,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E69" s="2" t="str">
         <f>IF(F69&lt;&gt;"",VLOOKUP(F69,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J69" s="3" t="str">
-        <f>IF(K69&lt;&gt;"",VLOOKUP(K69,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="3" t="str">
+        <f>IF(L69&lt;&gt;"",VLOOKUP(L69,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E70" s="2" t="str">
         <f>IF(F70&lt;&gt;"",VLOOKUP(F70,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J70" s="3" t="str">
-        <f>IF(K70&lt;&gt;"",VLOOKUP(K70,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="3" t="str">
+        <f>IF(L70&lt;&gt;"",VLOOKUP(L70,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E71" s="2" t="str">
         <f>IF(F71&lt;&gt;"",VLOOKUP(F71,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J71" s="3" t="str">
-        <f>IF(K71&lt;&gt;"",VLOOKUP(K71,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="3" t="str">
+        <f>IF(L71&lt;&gt;"",VLOOKUP(L71,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E72" s="2" t="str">
         <f>IF(F72&lt;&gt;"",VLOOKUP(F72,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J72" s="3" t="str">
-        <f>IF(K72&lt;&gt;"",VLOOKUP(K72,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="3" t="str">
+        <f>IF(L72&lt;&gt;"",VLOOKUP(L72,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E73" s="2" t="str">
         <f>IF(F73&lt;&gt;"",VLOOKUP(F73,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J73" s="3" t="str">
-        <f>IF(K73&lt;&gt;"",VLOOKUP(K73,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="3" t="str">
+        <f>IF(L73&lt;&gt;"",VLOOKUP(L73,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E74" s="2" t="str">
         <f>IF(F74&lt;&gt;"",VLOOKUP(F74,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J74" s="3" t="str">
-        <f>IF(K74&lt;&gt;"",VLOOKUP(K74,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="3" t="str">
+        <f>IF(L74&lt;&gt;"",VLOOKUP(L74,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E75" s="2" t="str">
         <f>IF(F75&lt;&gt;"",VLOOKUP(F75,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J75" s="3" t="str">
-        <f>IF(K75&lt;&gt;"",VLOOKUP(K75,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="3" t="str">
+        <f>IF(L75&lt;&gt;"",VLOOKUP(L75,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E76" s="2" t="str">
         <f>IF(F76&lt;&gt;"",VLOOKUP(F76,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J76" s="3" t="str">
-        <f>IF(K76&lt;&gt;"",VLOOKUP(K76,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="3" t="str">
+        <f>IF(L76&lt;&gt;"",VLOOKUP(L76,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E77" s="2" t="str">
         <f>IF(F77&lt;&gt;"",VLOOKUP(F77,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J77" s="3" t="str">
-        <f>IF(K77&lt;&gt;"",VLOOKUP(K77,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="3" t="str">
+        <f>IF(L77&lt;&gt;"",VLOOKUP(L77,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E78" s="2" t="str">
         <f>IF(F78&lt;&gt;"",VLOOKUP(F78,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J78" s="3" t="str">
-        <f>IF(K78&lt;&gt;"",VLOOKUP(K78,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="3" t="str">
+        <f>IF(L78&lt;&gt;"",VLOOKUP(L78,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E79" s="2" t="str">
         <f>IF(F79&lt;&gt;"",VLOOKUP(F79,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J79" s="3" t="str">
-        <f>IF(K79&lt;&gt;"",VLOOKUP(K79,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="3" t="str">
+        <f>IF(L79&lt;&gt;"",VLOOKUP(L79,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E80" s="2" t="str">
         <f>IF(F80&lt;&gt;"",VLOOKUP(F80,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J80" s="3" t="str">
-        <f>IF(K80&lt;&gt;"",VLOOKUP(K80,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="3" t="str">
+        <f>IF(L80&lt;&gt;"",VLOOKUP(L80,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E81" s="2" t="str">
         <f>IF(F81&lt;&gt;"",VLOOKUP(F81,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J81" s="3" t="str">
-        <f>IF(K81&lt;&gt;"",VLOOKUP(K81,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="3" t="str">
+        <f>IF(L81&lt;&gt;"",VLOOKUP(L81,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E82" s="2" t="str">
         <f>IF(F82&lt;&gt;"",VLOOKUP(F82,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J82" s="3" t="str">
-        <f>IF(K82&lt;&gt;"",VLOOKUP(K82,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="3" t="str">
+        <f>IF(L82&lt;&gt;"",VLOOKUP(L82,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E83" s="2" t="str">
         <f>IF(F83&lt;&gt;"",VLOOKUP(F83,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J83" s="3" t="str">
-        <f>IF(K83&lt;&gt;"",VLOOKUP(K83,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="3" t="str">
+        <f>IF(L83&lt;&gt;"",VLOOKUP(L83,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E84" s="2" t="str">
         <f>IF(F84&lt;&gt;"",VLOOKUP(F84,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J84" s="3" t="str">
-        <f>IF(K84&lt;&gt;"",VLOOKUP(K84,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="3" t="str">
+        <f>IF(L84&lt;&gt;"",VLOOKUP(L84,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E85" s="2" t="str">
         <f>IF(F85&lt;&gt;"",VLOOKUP(F85,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J85" s="3" t="str">
-        <f>IF(K85&lt;&gt;"",VLOOKUP(K85,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="3" t="str">
+        <f>IF(L85&lt;&gt;"",VLOOKUP(L85,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E86" s="2" t="str">
         <f>IF(F86&lt;&gt;"",VLOOKUP(F86,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J86" s="3" t="str">
-        <f>IF(K86&lt;&gt;"",VLOOKUP(K86,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="3" t="str">
+        <f>IF(L86&lt;&gt;"",VLOOKUP(L86,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E87" s="2" t="str">
         <f>IF(F87&lt;&gt;"",VLOOKUP(F87,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J87" s="3" t="str">
-        <f>IF(K87&lt;&gt;"",VLOOKUP(K87,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="3" t="str">
+        <f>IF(L87&lt;&gt;"",VLOOKUP(L87,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E88" s="2" t="str">
         <f>IF(F88&lt;&gt;"",VLOOKUP(F88,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J88" s="3" t="str">
-        <f>IF(K88&lt;&gt;"",VLOOKUP(K88,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="3" t="str">
+        <f>IF(L88&lt;&gt;"",VLOOKUP(L88,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E89" s="2" t="str">
         <f>IF(F89&lt;&gt;"",VLOOKUP(F89,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J89" s="3" t="str">
-        <f>IF(K89&lt;&gt;"",VLOOKUP(K89,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="3" t="str">
+        <f>IF(L89&lt;&gt;"",VLOOKUP(L89,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E90" s="2" t="str">
         <f>IF(F90&lt;&gt;"",VLOOKUP(F90,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J90" s="3" t="str">
-        <f>IF(K90&lt;&gt;"",VLOOKUP(K90,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="3" t="str">
+        <f>IF(L90&lt;&gt;"",VLOOKUP(L90,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E91" s="2" t="str">
         <f>IF(F91&lt;&gt;"",VLOOKUP(F91,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J91" s="3" t="str">
-        <f>IF(K91&lt;&gt;"",VLOOKUP(K91,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="3" t="str">
+        <f>IF(L91&lt;&gt;"",VLOOKUP(L91,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E92" s="2" t="str">
         <f>IF(F92&lt;&gt;"",VLOOKUP(F92,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J92" s="3" t="str">
-        <f>IF(K92&lt;&gt;"",VLOOKUP(K92,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="3" t="str">
+        <f>IF(L92&lt;&gt;"",VLOOKUP(L92,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E93" s="2" t="str">
         <f>IF(F93&lt;&gt;"",VLOOKUP(F93,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J93" s="3" t="str">
-        <f>IF(K93&lt;&gt;"",VLOOKUP(K93,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="3" t="str">
+        <f>IF(L93&lt;&gt;"",VLOOKUP(L93,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E94" s="2" t="str">
         <f>IF(F94&lt;&gt;"",VLOOKUP(F94,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J94" s="3" t="str">
-        <f>IF(K94&lt;&gt;"",VLOOKUP(K94,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="3" t="str">
+        <f>IF(L94&lt;&gt;"",VLOOKUP(L94,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E95" s="2" t="str">
         <f>IF(F95&lt;&gt;"",VLOOKUP(F95,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J95" s="3" t="str">
-        <f>IF(K95&lt;&gt;"",VLOOKUP(K95,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="3" t="str">
+        <f>IF(L95&lt;&gt;"",VLOOKUP(L95,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E96" s="2" t="str">
         <f>IF(F96&lt;&gt;"",VLOOKUP(F96,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J96" s="3" t="str">
-        <f>IF(K96&lt;&gt;"",VLOOKUP(K96,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="3" t="str">
+        <f>IF(L96&lt;&gt;"",VLOOKUP(L96,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E97" s="2" t="str">
         <f>IF(F97&lt;&gt;"",VLOOKUP(F97,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J97" s="3" t="str">
-        <f>IF(K97&lt;&gt;"",VLOOKUP(K97,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="3" t="str">
+        <f>IF(L97&lt;&gt;"",VLOOKUP(L97,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E98" s="2" t="str">
         <f>IF(F98&lt;&gt;"",VLOOKUP(F98,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J98" s="3" t="str">
-        <f>IF(K98&lt;&gt;"",VLOOKUP(K98,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="3" t="str">
+        <f>IF(L98&lt;&gt;"",VLOOKUP(L98,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E99" s="2" t="str">
         <f>IF(F99&lt;&gt;"",VLOOKUP(F99,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J99" s="3" t="str">
-        <f>IF(K99&lt;&gt;"",VLOOKUP(K99,DADOS!$D:$E,2,0),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="3" t="str">
+        <f>IF(L99&lt;&gt;"",VLOOKUP(L99,DADOS!$D:$E,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E100" s="2" t="str">
         <f>IF(F100&lt;&gt;"",VLOOKUP(F100,DADOS!$A:$B,2,0),"")</f>
         <v/>
       </c>
-      <c r="J100" s="3" t="str">
-        <f>IF(K100&lt;&gt;"",VLOOKUP(K100,DADOS!$D:$E,2,0),"")</f>
+      <c r="K100" s="3" t="str">
+        <f>IF(L100&lt;&gt;"",VLOOKUP(L100,DADOS!$D:$E,2,0),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H100" xr:uid="{E8E3075D-61DB-44A9-8144-679DDF5A72F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I100" xr:uid="{E8E3075D-61DB-44A9-8144-679DDF5A72F1}">
       <formula1>"PE,PB,RN,BA,SE,AL,CE,PI"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K100" xr:uid="{02C3F8B6-7299-42CD-80D5-4250D6498648}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L100" xr:uid="{02C3F8B6-7299-42CD-80D5-4250D6498648}">
       <formula1>"SIM,NÃO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D100" xr:uid="{DD8B4E74-F0C2-418C-8D1B-9945446DE89E}">
@@ -1812,6 +1833,10 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Arial"&amp;7&amp;K000000 ***Este documento está clasificado como PUBLICO por TELEFÓNICA.
+***This document is classified as PUBLIC by TELEFÓNICA.</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -1825,19 +1850,19 @@
           <x14:formula1>
             <xm:f>DADOS!$D2:$D10000</xm:f>
           </x14:formula1>
-          <xm:sqref>K2</xm:sqref>
+          <xm:sqref>L2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{93A473EB-241A-4B74-8222-BAD160413754}">
+          <x14:formula1>
+            <xm:f>DADOS!$I2:$I1000</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{679344CC-FE17-49C4-8CC0-14E79D4A7D19}">
           <x14:formula1>
             <xm:f>DADOS!$G2:$G10000</xm:f>
           </x14:formula1>
           <xm:sqref>D2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{93A473EB-241A-4B74-8222-BAD160413754}">
-          <x14:formula1>
-            <xm:f>DADOS!$I2:$I1000</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1853,9 +1878,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1872,7 +1897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1892,7 +1917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1912,7 +1937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1926,7 +1951,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1940,7 +1965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1954,7 +1979,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1968,7 +1993,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1982,7 +2007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1993,7 +2018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2001,7 +2026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2009,7 +2034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2025,7 +2050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2033,7 +2058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2041,7 +2066,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2049,7 +2074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2057,7 +2082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -2065,7 +2090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2073,7 +2098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -2081,7 +2106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2089,7 +2114,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2100,10 +2125,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="F19X/DAxomGOiPl5e3/gR6IdJjXlxBG6NAtJVodPUS/Jz7aqgyQa162/J0Jy+8tQOkUPoNH3uGsrypDhRVVXYQ==" saltValue="MRdWwsACScyjQgVSQBwKqA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Arial"&amp;7&amp;K000000 ***Este documento está clasificado como PUBLICO por TELEFÓNICA.
+***This document is classified as PUBLIC by TELEFÓNICA.</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100421D3DE04D9BE748995368097EF9BB96" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4f27219fd59605f926c9bc63e215239e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bdb1dba8-fec7-4287-bf3e-36a99c68d6ae" xmlns:ns3="9ee4a531-a89b-45df-ae52-3d445cfb3f49" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b17c03802ba9a2af284eaae4217c69f" ns2:_="" ns3:_="">
     <xsd:import namespace="bdb1dba8-fec7-4287-bf3e-36a99c68d6ae"/>
@@ -2320,16 +2358,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821BC8C5-0082-49DF-B658-C2EF7E2AB2B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E2591B3-4DE1-4BC0-92A1-5046F244A075}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2348,10 +2385,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821BC8C5-0082-49DF-B658-C2EF7E2AB2B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e65bd4d2-aa7c-445f-9ef8-222ebb1d2b43}" enabled="1" method="Privileged" siteId="{9744600e-3e04-492e-baa1-25ec245c6f10}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>